<commit_message>
placing info on page
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26122"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-26260" yWindow="5280" windowWidth="24000" windowHeight="16420"/>
+    <workbookView xWindow="13180" yWindow="0" windowWidth="11360" windowHeight="14240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -137,57 +137,27 @@
     <t>Image File Path</t>
   </si>
   <si>
-    <t>Merri</t>
-  </si>
-  <si>
     <t>/abc/abc.com</t>
   </si>
   <si>
     <t>African</t>
   </si>
   <si>
-    <t>Africa</t>
-  </si>
-  <si>
     <t>Boxing</t>
   </si>
   <si>
-    <t>Heavy</t>
-  </si>
-  <si>
-    <t>5'10"</t>
-  </si>
-  <si>
-    <t>phili</t>
-  </si>
-  <si>
     <t>horse</t>
   </si>
   <si>
     <t>fight</t>
   </si>
   <si>
-    <t>compton</t>
-  </si>
-  <si>
-    <t>bubba</t>
-  </si>
-  <si>
-    <t>lengthy</t>
-  </si>
-  <si>
-    <t>not</t>
-  </si>
-  <si>
     <t>street</t>
   </si>
   <si>
     <t>medium</t>
   </si>
   <si>
-    <t>you know</t>
-  </si>
-  <si>
     <t>yep</t>
   </si>
   <si>
@@ -209,13 +179,55 @@
     <t>vinyl</t>
   </si>
   <si>
-    <t>Category Id</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t>Athelete Id</t>
+  </si>
+  <si>
+    <t>Ronda Rousey</t>
+  </si>
+  <si>
+    <t>5'7"</t>
+  </si>
+  <si>
+    <t>Glendale Fighting Club</t>
+  </si>
+  <si>
+    <t>Women's Bantamweight</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Rowdy</t>
+  </si>
+  <si>
+    <t>Orthodox</t>
+  </si>
+  <si>
+    <t>Judo</t>
+  </si>
+  <si>
+    <t>UFC</t>
+  </si>
+  <si>
+    <t>UFClogo.jpg</t>
+  </si>
+  <si>
+    <t>2-0</t>
+  </si>
+  <si>
+    <t>9-0</t>
+  </si>
+  <si>
+    <t>2/1/1987</t>
+  </si>
+  <si>
+    <t>United States</t>
   </si>
 </sst>
 </file>
@@ -283,7 +295,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -583,7 +595,9 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -592,15 +606,15 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B2" s="1">
         <v>1111</v>
@@ -611,7 +625,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -619,7 +633,7 @@
         <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -627,7 +641,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -635,7 +649,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -643,7 +657,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -651,7 +665,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -659,7 +673,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -667,7 +681,7 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>200</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -675,7 +689,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -683,7 +697,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -691,7 +705,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -699,15 +713,15 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:2" s="1" customFormat="1">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="4">
-        <v>40544</v>
+      <c r="B15" s="4" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -715,7 +729,7 @@
         <v>36</v>
       </c>
       <c r="B16">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -723,7 +737,7 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -731,15 +745,15 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B19" t="s">
-        <v>50</v>
+      <c r="B19">
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -747,7 +761,7 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -755,7 +769,7 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -763,7 +777,7 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -771,7 +785,7 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -779,7 +793,7 @@
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -787,7 +801,7 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -795,7 +809,7 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -803,7 +817,7 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -811,7 +825,7 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -819,7 +833,7 @@
         <v>24</v>
       </c>
       <c r="B29">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -827,7 +841,7 @@
         <v>25</v>
       </c>
       <c r="B30">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -835,23 +849,23 @@
         <v>26</v>
       </c>
       <c r="B31">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B32">
-        <v>5</v>
+      <c r="B32" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B33">
-        <v>5</v>
+      <c r="B33" s="4" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -875,7 +889,7 @@
         <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -891,7 +905,7 @@
         <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -899,7 +913,7 @@
         <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -913,6 +927,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="B32:B33" twoDigitTextYear="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>